<commit_message>
first push for hybrid framwork
</commit_message>
<xml_diff>
--- a/data/Excel.xlsx
+++ b/data/Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monjoy/IdeaProjects/TeamPython_HybridFrameWork/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flyer\IdeaProjects\TeamPython_HybridFrameWork\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7349896-C0DE-0042-BDF1-2C8C6F93E11D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D3B17E-A8BB-42A7-A52A-408259675F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16620" xr2:uid="{D4DC3308-5999-8347-8F01-CB7EC91F937E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D4DC3308-5999-8347-8F01-CB7EC91F937E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,152 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+  <si>
+    <t>khan23@gmail.com</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>khan234@gmail.com</t>
+  </si>
+  <si>
+    <t>abc12</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Blouses</t>
+  </si>
+  <si>
+    <t>Customer service</t>
+  </si>
+  <si>
+    <t>Hey, everything is good</t>
+  </si>
+  <si>
+    <t>CUSTOMER SERVICE - CONTACT US</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?controller=order</t>
+  </si>
+  <si>
+    <t>MY ADDRESSES</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>YOUR ADDRESSES</t>
+  </si>
+  <si>
+    <t>East 56</t>
+  </si>
+  <si>
+    <t>Queens</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>348 309 3487</t>
+  </si>
+  <si>
+    <t>East 7th</t>
+  </si>
+  <si>
+    <t>11334</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?controller=address</t>
+  </si>
+  <si>
+    <t>Your addresses are listed below.</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?controller=history</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?id_product=1&amp;controller=product</t>
+  </si>
+  <si>
+    <t>Shipments and returns</t>
+  </si>
+  <si>
+    <t>Legal</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?id_cms=3&amp;controller=cms</t>
+  </si>
+  <si>
+    <t>OUR TEAM</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?id_cms=5&amp;controller=cms</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?controller=stores</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?controller=identity</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>1993</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?id_category=3&amp;controller=category</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?controller=prices-drop</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?controller=new-products</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?controller=best-sales</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?controller=contact</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?id_cms=4&amp;controller=cms</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php?controller=sitemap</t>
+  </si>
+  <si>
+    <t>T-shirts</t>
+  </si>
+  <si>
+    <t>summer dresses</t>
+  </si>
+  <si>
+    <t>evening dresses</t>
+  </si>
+  <si>
+    <t>casual dresses</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -34,16 +177,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF555454"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -51,14 +226,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD6D4D4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -371,12 +596,223 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB82815A-94AC-2C4A-ABB9-0509CC31F7BD}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" width="18.75" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="36.83203125" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24.58203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="16" thickBot="1">
+      <c r="H1" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16" thickBot="1">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" thickBot="1">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="31.5" thickBot="1">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="31.5" thickBot="1">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="47" thickBot="1">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="47" thickBot="1">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="46.5">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="46.5">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="46.5">
+      <c r="E10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="46.5">
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="46.5">
+      <c r="E12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="46.5">
+      <c r="G13" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="46.5">
+      <c r="G14" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="46.5">
+      <c r="G15" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{696799B8-95B7-4667-80ED-420E9D9BBAAD}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{E6DDB5B6-9973-4694-89D6-1F5DCA3BCD84}"/>
+    <hyperlink ref="A6" r:id="rId3" xr:uid="{61288B89-60CB-4EC4-AB5D-073FEE884391}"/>
+    <hyperlink ref="A8" r:id="rId4" xr:uid="{1E122395-90C7-414D-A434-901D5CA9B5D1}"/>
+    <hyperlink ref="E8" r:id="rId5" xr:uid="{B766EF86-C4A1-4D07-9775-144E43791EEF}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{054D6D75-0945-4066-A284-40AC8C699E4D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>